<commit_message>
UPDATE ROAD_TYPE FR LABEL
</commit_message>
<xml_diff>
--- a/04-DOCS/XLS/Waze for Cities Data _ Data Dictionary for Alerts, Jams, and Irregularities.xlsx
+++ b/04-DOCS/XLS/Waze for Cities Data _ Data Dictionary for Alerts, Jams, and Irregularities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allfab\Downloads\Waze\04-DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Allfab\Documents\eWorking\Waze\04-DOCS\XLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB171686-7C90-4230-92A5-5C45E8A145E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A223C341-3065-4904-BB9D-62D05535025F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="285" windowWidth="28110" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="285" windowWidth="28110" windowHeight="16065" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="232">
   <si>
     <t>Reference guide for alerts, jams and irregularities</t>
   </si>
@@ -690,6 +690,57 @@
   </si>
   <si>
     <t>TEMPS DANGEREUX - INONDATION</t>
+  </si>
+  <si>
+    <t>RUE</t>
+  </si>
+  <si>
+    <t>RUE PRINCIPALE</t>
+  </si>
+  <si>
+    <t>AUTOROUTE</t>
+  </si>
+  <si>
+    <t>RAMPE</t>
+  </si>
+  <si>
+    <t>PISTE</t>
+  </si>
+  <si>
+    <t>RUE SECONDAIRE</t>
+  </si>
+  <si>
+    <t>SENTIERS 4X4</t>
+  </si>
+  <si>
+    <t>PASSERELLE</t>
+  </si>
+  <si>
+    <t>PIÉTON</t>
+  </si>
+  <si>
+    <t>SORTIR</t>
+  </si>
+  <si>
+    <t>TRAVERSÉE EN FERRY</t>
+  </si>
+  <si>
+    <t>ESCALIER</t>
+  </si>
+  <si>
+    <t>CHEMIN PRIVÉ</t>
+  </si>
+  <si>
+    <t>CHEMINS DE FER</t>
+  </si>
+  <si>
+    <t>PISTE/VOIE DE CIRCULATION</t>
+  </si>
+  <si>
+    <t>ROUTE DU PARKING</t>
+  </si>
+  <si>
+    <t>SERVICE ROUTIER</t>
   </si>
 </sst>
 </file>
@@ -6667,7 +6718,7 @@
   </sheetPr>
   <dimension ref="A1:H1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -13079,14 +13130,15 @@
   </sheetPr>
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="102" customHeight="1">
@@ -13140,7 +13192,9 @@
       <c r="B4" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="32" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="21.75">
       <c r="A5" s="39">
@@ -13149,7 +13203,9 @@
       <c r="B5" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="32" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="21.75">
       <c r="A6" s="39">
@@ -13158,7 +13214,9 @@
       <c r="B6" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="32" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="21.75">
       <c r="A7" s="39">
@@ -13167,7 +13225,9 @@
       <c r="B7" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="32" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="21.75">
       <c r="A8" s="39">
@@ -13176,7 +13236,9 @@
       <c r="B8" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="32" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="21.75">
       <c r="A9" s="39">
@@ -13185,7 +13247,9 @@
       <c r="B9" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="21.75">
       <c r="A10" s="39">
@@ -13194,7 +13258,9 @@
       <c r="B10" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="32" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="21.75">
       <c r="A11" s="39">
@@ -13203,7 +13269,9 @@
       <c r="B11" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="32" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="21.75">
       <c r="A12" s="39">
@@ -13212,7 +13280,9 @@
       <c r="B12" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="32"/>
+      <c r="C12" s="32" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="21.75">
       <c r="A13" s="39">
@@ -13221,7 +13291,9 @@
       <c r="B13" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="32"/>
+      <c r="C13" s="32" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="21.75">
       <c r="A14" s="39">
@@ -13230,7 +13302,9 @@
       <c r="B14" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="C14" s="32"/>
+      <c r="C14" s="32" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="21.75">
       <c r="A15" s="39">
@@ -13239,7 +13313,9 @@
       <c r="B15" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="32" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="21.75">
       <c r="A16" s="39">
@@ -13248,7 +13324,9 @@
       <c r="B16" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="32"/>
+      <c r="C16" s="32" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="21.75">
       <c r="A17" s="39">
@@ -13257,7 +13335,9 @@
       <c r="B17" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C17" s="32"/>
+      <c r="C17" s="32" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="21.75">
       <c r="A18" s="39">
@@ -13266,7 +13346,9 @@
       <c r="B18" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="C18" s="32"/>
+      <c r="C18" s="32" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="21.75">
       <c r="A19" s="39">
@@ -13275,7 +13357,9 @@
       <c r="B19" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="32"/>
+      <c r="C19" s="32" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="21.75">
       <c r="A20" s="39">
@@ -13284,7 +13368,9 @@
       <c r="B20" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="32" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="21.75">
       <c r="A21" s="39">
@@ -13293,7 +13379,9 @@
       <c r="B21" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="C21" s="32"/>
+      <c r="C21" s="32" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="21.75">
       <c r="A22" s="39">
@@ -13302,7 +13390,9 @@
       <c r="B22" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="32"/>
+      <c r="C22" s="32" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A3:B22" xr:uid="{00000000-0009-0000-0000-000004000000}">

</xml_diff>